<commit_message>
Tablas,Doc y Reqs Actualizados
</commit_message>
<xml_diff>
--- a/Docs/Tablas Reto 3.xlsx
+++ b/Docs/Tablas Reto 3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/s_rodriguez63_uniandes_edu_co/Documents/Sicua Plus Andes/Sicua Plus Andes/Tercer Semestre/Estructuras Datos y Algoritmos/Retos/Reto #3/Reto3-G13/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{8C875C38-3874-4A92-B7A0-531E2D3692E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22EE0602-A01C-42BE-9054-124380E32D71}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="13_ncr:1_{8C875C38-3874-4A92-B7A0-531E2D3692E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{425B1FDC-480D-4EBD-9271-6FF606BE0B90}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Reto" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Porcentaje de la muestra [pct]</t>
   </si>
@@ -126,21 +126,6 @@
   </si>
   <si>
     <t>Req 3, Req 5 y Req 6</t>
-  </si>
-  <si>
-    <t>31.25</t>
-  </si>
-  <si>
-    <t>8359.38</t>
-  </si>
-  <si>
-    <t>22296.88</t>
-  </si>
-  <si>
-    <t>10375.0</t>
-  </si>
-  <si>
-    <t>33843.75</t>
   </si>
 </sst>
 </file>
@@ -258,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -291,6 +276,7 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -306,7 +292,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1779,28 +1773,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>62.5</c:v>
+                  <c:v>15.62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>359.38</c:v>
+                  <c:v>78.12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>828.12</c:v>
+                  <c:v>140.62</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1765.62</c:v>
+                  <c:v>281.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2718.75</c:v>
+                  <c:v>468.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4859.38</c:v>
+                  <c:v>890.62</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1406.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1796.88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2942,10 +2936,10 @@
                   <c:v>31.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>31.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>31.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3496,28 +3490,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>125</c:v>
+                  <c:v>31.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2281.25</c:v>
+                  <c:v>46.88</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7812.5</c:v>
+                  <c:v>62.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32812.5</c:v>
+                  <c:v>46.88</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79671.88</c:v>
+                  <c:v>93.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14140.62</c:v>
+                  <c:v>62.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>62.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>93.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8325,7 +8319,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3D4D373F-B89D-476A-916E-D6B8B50B0AC1}">
   <sheetPr codeName="Gráfico2"/>
   <sheetViews>
-    <sheetView zoomScale="119" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8336,7 +8330,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{39C68510-AE01-4761-A7FB-5F1B76E923F7}">
   <sheetPr codeName="Gráfico3"/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="92" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8347,7 +8341,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{C0D6BB1E-4928-4857-A0CD-C818D0A5A6F2}">
   <sheetPr codeName="Gráfico4"/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="92" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8358,7 +8352,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B3AE6AD4-6EB7-44ED-A987-5D4A68E7E10B}">
   <sheetPr codeName="Gráfico5"/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="92" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8369,7 +8363,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{F5354549-71FD-5049-997E-1F059B8A05CE}">
   <sheetPr codeName="Gráfico6"/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="92" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8380,7 +8374,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{A7ACBD8B-9E65-0D43-AFC7-473A72AFA26E}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="92" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8391,7 +8385,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{76E53AE1-139A-4B4B-981B-2C1C7E11A6C6}">
   <sheetPr codeName="Gráfico8"/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="92" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8402,7 +8396,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8668550" cy="6291303"/>
+    <xdr:ext cx="8670151" cy="6288101"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -8435,7 +8429,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6293013"/>
+    <xdr:ext cx="8680174" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -8468,7 +8462,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6293013"/>
+    <xdr:ext cx="8680174" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -8501,7 +8495,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6293013"/>
+    <xdr:ext cx="8680174" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -8534,7 +8528,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6293013"/>
+    <xdr:ext cx="8680174" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -8567,7 +8561,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6293013"/>
+    <xdr:ext cx="8680174" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -8600,7 +8594,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6293013"/>
+    <xdr:ext cx="8680174" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -8949,8 +8943,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -9006,7 +9000,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="9">
-        <v>62.5</v>
+        <v>15.62</v>
       </c>
       <c r="F2" s="9">
         <v>0</v>
@@ -9015,9 +9009,9 @@
         <v>0</v>
       </c>
       <c r="H2" s="9">
-        <v>125</v>
-      </c>
-      <c r="I2" s="9">
+        <v>31.25</v>
+      </c>
+      <c r="I2" s="18">
         <v>109.38</v>
       </c>
     </row>
@@ -9035,7 +9029,7 @@
         <v>15.62</v>
       </c>
       <c r="E3" s="10">
-        <v>359.38</v>
+        <v>78.12</v>
       </c>
       <c r="F3" s="10">
         <v>31.25</v>
@@ -9044,9 +9038,9 @@
         <v>15.62</v>
       </c>
       <c r="H3" s="10">
-        <v>2281.25</v>
-      </c>
-      <c r="I3" s="10">
+        <v>46.88</v>
+      </c>
+      <c r="I3" s="19">
         <v>359.38</v>
       </c>
     </row>
@@ -9064,7 +9058,7 @@
         <v>46.88</v>
       </c>
       <c r="E4" s="9">
-        <v>828.12</v>
+        <v>140.62</v>
       </c>
       <c r="F4" s="9">
         <v>46.88</v>
@@ -9073,9 +9067,9 @@
         <v>0</v>
       </c>
       <c r="H4" s="9">
-        <v>7812.5</v>
-      </c>
-      <c r="I4" s="9">
+        <v>62.5</v>
+      </c>
+      <c r="I4" s="18">
         <v>703.12</v>
       </c>
     </row>
@@ -9093,7 +9087,7 @@
         <v>93.75</v>
       </c>
       <c r="E5" s="10">
-        <v>1765.62</v>
+        <v>281.25</v>
       </c>
       <c r="F5" s="10">
         <v>109.38</v>
@@ -9102,9 +9096,9 @@
         <v>15.62</v>
       </c>
       <c r="H5" s="10">
-        <v>32812.5</v>
-      </c>
-      <c r="I5" s="10">
+        <v>46.88</v>
+      </c>
+      <c r="I5" s="19">
         <v>1234.3800000000001</v>
       </c>
     </row>
@@ -9122,7 +9116,7 @@
         <v>156.25</v>
       </c>
       <c r="E6" s="9">
-        <v>2718.75</v>
+        <v>468.75</v>
       </c>
       <c r="F6" s="9">
         <v>171.88</v>
@@ -9131,9 +9125,9 @@
         <v>15.62</v>
       </c>
       <c r="H6" s="9">
-        <v>79671.88</v>
-      </c>
-      <c r="I6" s="9">
+        <v>93.75</v>
+      </c>
+      <c r="I6" s="18">
         <v>1750</v>
       </c>
     </row>
@@ -9151,7 +9145,7 @@
         <v>281.25</v>
       </c>
       <c r="E7" s="10">
-        <v>4859.38</v>
+        <v>890.62</v>
       </c>
       <c r="F7" s="10">
         <v>296.88</v>
@@ -9160,9 +9154,9 @@
         <v>31.25</v>
       </c>
       <c r="H7" s="10">
-        <v>14140.62</v>
-      </c>
-      <c r="I7" s="10">
+        <v>62.5</v>
+      </c>
+      <c r="I7" s="19">
         <v>2843.75</v>
       </c>
     </row>
@@ -9179,19 +9173,19 @@
       <c r="D8" s="9">
         <v>453.12</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>26</v>
+      <c r="E8" s="9">
+        <v>1406.25</v>
       </c>
       <c r="F8" s="9">
         <v>500</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" s="9">
+      <c r="G8" s="9">
+        <v>31.25</v>
+      </c>
+      <c r="H8" s="9">
+        <v>62.5</v>
+      </c>
+      <c r="I8" s="18">
         <v>4390.62</v>
       </c>
     </row>
@@ -9208,27 +9202,27 @@
       <c r="D9" s="11">
         <v>578.12</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>28</v>
+      <c r="E9" s="11">
+        <v>1796.88</v>
       </c>
       <c r="F9" s="11">
         <v>656.25</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="11">
+      <c r="G9" s="11">
+        <v>31.25</v>
+      </c>
+      <c r="H9" s="11">
+        <v>93.75</v>
+      </c>
+      <c r="I9" s="20">
         <v>5250</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="15"/>
+      <c r="B11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="28.8">
       <c r="A12" s="7" t="s">
@@ -9237,7 +9231,7 @@
       <c r="B12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="17"/>
+      <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="7" t="s">
@@ -9246,6 +9240,7 @@
       <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="7" t="s">
@@ -9264,10 +9259,10 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="16"/>
+      <c r="B17" s="17"/>
     </row>
     <row r="18" spans="1:2" ht="28.8">
       <c r="A18" s="7" t="s">
@@ -9302,10 +9297,10 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="36" customHeight="1">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="13"/>
+      <c r="B23" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -9324,6 +9319,115 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743">
+      <UserInfo>
+        <DisplayName>Carlos Andres Lozano Garzon</DisplayName>
+        <AccountId>13</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Dario Ernesto Correal Torres</DisplayName>
+        <AccountId>15</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Mario  Fernando De la rosa Rosero</DisplayName>
+        <AccountId>16</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Christian Camilo Aparicio Baquen</DisplayName>
+        <AccountId>50</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Arturo Henao Chaparro</DisplayName>
+        <AccountId>48</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Luis Esteban Florez Salamanca</DisplayName>
+        <AccountId>33</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ivan David Salazar Cardenas</DisplayName>
+        <AccountId>52</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Juan Carlos Marin Morales</DisplayName>
+        <AccountId>53</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Sofia Duque Gomez</DisplayName>
+        <AccountId>60</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Andres Felipe Romero Brand</DisplayName>
+        <AccountId>91</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Lindsay Vanessa Pinto Morato</DisplayName>
+        <AccountId>92</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Miguel Angel Acosta Walteros</DisplayName>
+        <AccountId>94</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Juan David Diaz Ipuz</DisplayName>
+        <AccountId>90</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Lily Aitana valentina Duque Chavez</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Isaac David Bermudez Lara</DisplayName>
+        <AccountId>95</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Daniel Alejandro Angel Fuertes</DisplayName>
+        <AccountId>55</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jeniffer Liliam Mendoza Espinosa</DisplayName>
+        <AccountId>97</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kevin Cohen Solano</DisplayName>
+        <AccountId>93</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Cesar Luis Moreno Gonzalez</DisplayName>
+        <AccountId>96</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jose Cristobal Arroyo Castellanos</DisplayName>
+        <AccountId>54</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010023858CF01A2EF24688B692775F4C60A4" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="6ca5caf3e573104b48cd489fb7ebf238">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="164883f8-7691-4ecf-b54a-664c0d0edefe" xmlns:ns3="85e30bcc-d76c-4413-8e4d-2dce22fb0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f8ff97dc266d6a6a16fe4e7cad907b60" ns2:_="" ns3:_="">
     <xsd:import namespace="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -9540,115 +9644,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743">
-      <UserInfo>
-        <DisplayName>Carlos Andres Lozano Garzon</DisplayName>
-        <AccountId>13</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Dario Ernesto Correal Torres</DisplayName>
-        <AccountId>15</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Mario  Fernando De la rosa Rosero</DisplayName>
-        <AccountId>16</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Christian Camilo Aparicio Baquen</DisplayName>
-        <AccountId>50</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Arturo Henao Chaparro</DisplayName>
-        <AccountId>48</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Luis Esteban Florez Salamanca</DisplayName>
-        <AccountId>33</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ivan David Salazar Cardenas</DisplayName>
-        <AccountId>52</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Juan Carlos Marin Morales</DisplayName>
-        <AccountId>53</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Sofia Duque Gomez</DisplayName>
-        <AccountId>60</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Andres Felipe Romero Brand</DisplayName>
-        <AccountId>91</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Lindsay Vanessa Pinto Morato</DisplayName>
-        <AccountId>92</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Miguel Angel Acosta Walteros</DisplayName>
-        <AccountId>94</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Juan David Diaz Ipuz</DisplayName>
-        <AccountId>90</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Lily Aitana valentina Duque Chavez</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Isaac David Bermudez Lara</DisplayName>
-        <AccountId>95</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Daniel Alejandro Angel Fuertes</DisplayName>
-        <AccountId>55</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jeniffer Liliam Mendoza Espinosa</DisplayName>
-        <AccountId>97</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kevin Cohen Solano</DisplayName>
-        <AccountId>93</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Cesar Luis Moreno Gonzalez</DisplayName>
-        <AccountId>96</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jose Cristobal Arroyo Castellanos</DisplayName>
-        <AccountId>54</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -9659,6 +9654,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3198979-0B27-4D27-8331-28B531282E06}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9677,23 +9689,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
   <ds:schemaRefs>

</xml_diff>